<commit_message>
Updating weak scaling plot with 4096 node run.
</commit_message>
<xml_diff>
--- a/scaling/PeleC_Scaling.xlsx
+++ b/scaling/PeleC_Scaling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrood/Documents/Combustion/PeleStuff/scaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72B4EEA-7612-1F4A-BEDD-618558066C27}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC264AD-272F-3846-A606-AE0D00F2D949}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="5680" windowWidth="29580" windowHeight="18980" xr2:uid="{02F37BB5-5E65-AC45-9AE5-613D8DDC46D9}"/>
+    <workbookView xWindow="12180" yWindow="6320" windowWidth="29580" windowHeight="18980" xr2:uid="{02F37BB5-5E65-AC45-9AE5-613D8DDC46D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$7:$B$11</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>PeleC Weak Scaling PMF Case 6/12/2018</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>PeleC I/O Statistics with Burst Buffer</t>
+  </si>
+  <si>
+    <t>Parallel Efficiency</t>
   </si>
 </sst>
 </file>
@@ -186,7 +189,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
+              <a:t> KNL </a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -229,7 +232,7 @@
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$D$6</c:f>
@@ -317,7 +320,7 @@
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="0"/>
           <c:tx>
             <c:v>KNL run time</c:v>
           </c:tx>
@@ -367,7 +370,7 @@
                   <c:v>2048</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8192</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -394,7 +397,7 @@
                   <c:v>1300.7819469999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1362.7958822000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -406,11 +409,23 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
-            <c:v>Haswell run time</c:v>
+            <c:v>Parallel Efficiency</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -444,42 +459,54 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$16:$A$19</c:f>
+              <c:f>Sheet1!$B$7:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>512</c:v>
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>524288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$19</c:f>
+              <c:f>Sheet1!$E$7:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>990.27273400000001</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1009.7371450000001</c:v>
+                  <c:v>0.98135519198732224</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1048.1402169999999</c:v>
+                  <c:v>0.97151224101829248</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1079.18695</c:v>
+                  <c:v>0.94867419807226705</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.93821290479518016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89551958949997479</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -487,7 +514,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0CD8-8942-A450-8CB7EDF3B55D}"/>
+              <c16:uniqueId val="{00000000-EFFE-1A4F-9D29-396888B93453}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -499,113 +526,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1429419744"/>
-        <c:axId val="1460227696"/>
-      </c:scatterChart>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Threads</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$7:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32768</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>262144</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1048576</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$7:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1220.4104090000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1243.597037</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1256.1966359999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1286.437864</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1300.7819469999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-54EE-9441-BE8A-CC53C6988613}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1671883183"/>
-        <c:axId val="1671833167"/>
+        <c:axId val="1632828352"/>
+        <c:axId val="1618725392"/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="1429419744"/>
@@ -833,22 +755,106 @@
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1671833167"/>
+        <c:axId val="1618725392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Parallel Efficiency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1671883183"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1632828352"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1671883183"/>
+        <c:axId val="1632828352"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -877,13 +883,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Threads on KNL (32 MPI ranks</a:t>
+                  <a:t>Threads</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> per socket, 4 threads per rank)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -947,7 +948,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1671833167"/>
+        <c:crossAx val="1618725392"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -961,16 +962,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.3708925754826965"/>
-          <c:y val="0.94230742896268405"/>
-          <c:w val="0.40073266376144789"/>
-          <c:h val="3.7625681405208972E-2"/>
-        </c:manualLayout>
-      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4542,7 +4533,7 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4553,17 +4544,17 @@
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
@@ -4571,7 +4562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4584,8 +4575,11 @@
       <c r="D6" t="s">
         <v>4</v>
       </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4598,8 +4592,12 @@
       <c r="D7">
         <v>1344.514488</v>
       </c>
+      <c r="E7">
+        <f>$C$7/C7</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -4612,8 +4610,12 @@
       <c r="D8">
         <v>1354.4657010000001</v>
       </c>
+      <c r="E8">
+        <f t="shared" ref="E8:E12" si="0">$C$7/C8</f>
+        <v>0.98135519198732224</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>32</v>
       </c>
@@ -4626,8 +4628,12 @@
       <c r="D9">
         <v>1393.417893</v>
       </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.97151224101829248</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>256</v>
       </c>
@@ -4640,8 +4646,12 @@
       <c r="D10">
         <v>1390.407387</v>
       </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.94867419807226705</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2048</v>
       </c>
@@ -4654,24 +4664,32 @@
       <c r="D11">
         <v>1408.424583</v>
       </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.93821290479518016</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>8192</v>
+        <v>4096</v>
       </c>
       <c r="B12">
-        <v>1048576</v>
+        <v>524288</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1362.7958822000001</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.89551958949997479</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -4679,7 +4697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -4770,7 +4788,7 @@
         <v>2.5740230080000002</v>
       </c>
       <c r="F35">
-        <f t="shared" ref="F35:F37" si="0">C35/E35</f>
+        <f t="shared" ref="F35:F37" si="1">C35/E35</f>
         <v>5.8274537381291349</v>
       </c>
     </row>
@@ -4788,7 +4806,7 @@
         <v>11.02806807</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.427937084722764</v>
       </c>
     </row>
@@ -4806,7 +4824,7 @@
         <v>81.590362069999998</v>
       </c>
       <c r="F37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.190047167785536</v>
       </c>
     </row>
@@ -4864,7 +4882,7 @@
         <v>3.8251938820000002</v>
       </c>
       <c r="F43">
-        <f t="shared" ref="F43:F45" si="1">C43/E43</f>
+        <f t="shared" ref="F43:F45" si="2">C43/E43</f>
         <v>7.8427397212908119</v>
       </c>
     </row>
@@ -4882,7 +4900,7 @@
         <v>15.325423000000001</v>
       </c>
       <c r="F44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15.268746578805688</v>
       </c>
     </row>
@@ -4900,7 +4918,7 @@
         <v>130.34055499999999</v>
       </c>
       <c r="F45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14.577197404138721</v>
       </c>
     </row>
@@ -4963,7 +4981,7 @@
         <v>1.732409954</v>
       </c>
       <c r="F55">
-        <f t="shared" ref="F55:F56" si="2">C55/E55</f>
+        <f t="shared" ref="F55:F56" si="3">C55/E55</f>
         <v>8.6584586779625496</v>
       </c>
     </row>
@@ -4981,7 +4999,7 @@
         <v>5.3756639960000001</v>
       </c>
       <c r="F56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21.392706107667969</v>
       </c>
     </row>
@@ -5057,7 +5075,7 @@
         <v>2.7114350800000002</v>
       </c>
       <c r="F63">
-        <f t="shared" ref="F63:F64" si="3">C63/E63</f>
+        <f t="shared" ref="F63:F64" si="4">C63/E63</f>
         <v>11.064251628698408</v>
       </c>
     </row>
@@ -5075,7 +5093,7 @@
         <v>6.2747130389999999</v>
       </c>
       <c r="F64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37.292542072536364</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating weak scaling plot.
</commit_message>
<xml_diff>
--- a/scaling/PeleC_Scaling.xlsx
+++ b/scaling/PeleC_Scaling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrood/Documents/Combustion/PeleStuff/scaling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC264AD-272F-3846-A606-AE0D00F2D949}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C463F5-B899-194B-89E1-7359C4AA7C78}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="6320" windowWidth="29580" windowHeight="18980" xr2:uid="{02F37BB5-5E65-AC45-9AE5-613D8DDC46D9}"/>
+    <workbookView xWindow="10180" yWindow="5940" windowWidth="29580" windowHeight="18980" xr2:uid="{02F37BB5-5E65-AC45-9AE5-613D8DDC46D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>PeleC Weak Scaling PMF Case 6/12/2018</t>
   </si>
@@ -84,7 +84,10 @@
     <t>PeleC I/O Statistics with Burst Buffer</t>
   </si>
   <si>
-    <t>Parallel Efficiency</t>
+    <t>Parallel efficiency</t>
+  </si>
+  <si>
+    <t>KNL run time</t>
   </si>
 </sst>
 </file>
@@ -185,11 +188,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>PeleC Weak Scaling on Cori</a:t>
+              <a:t>PeleC Weak Scaling on Cori KNL - ~4 Million Cells Per Socket</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> KNL </a:t>
+              <a:t> </a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -322,7 +325,15 @@
           <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>KNL run time</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KNL run time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -417,22 +428,30 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:axId val="1429419744"/>
+        <c:axId val="1460227696"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="0"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Parallel Efficiency</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$E$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Parallel efficiency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -443,15 +462,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -514,7 +529,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EFFE-1A4F-9D29-396888B93453}"/>
+              <c16:uniqueId val="{00000000-C29E-8C44-A2A7-67D8DF2D9790}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -526,8 +541,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1632828352"/>
-        <c:axId val="1618725392"/>
+        <c:axId val="588732927"/>
+        <c:axId val="589211951"/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="1429419744"/>
@@ -559,15 +574,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Sockets (</a:t>
+                  <a:t>CPU Sockets</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>~4 Million Grid Cells Per Node)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -645,7 +653,7 @@
         <c:axId val="1460227696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1600"/>
+          <c:max val="1800"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -755,7 +763,7 @@
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1618725392"/>
+        <c:axId val="589211951"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -849,12 +857,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1632828352"/>
+        <c:crossAx val="588732927"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1632828352"/>
+        <c:axId val="588732927"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -948,7 +956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1618725392"/>
+        <c:crossAx val="589211951"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -962,6 +970,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.3708925754826965"/>
+          <c:y val="0.94230742896268405"/>
+          <c:w val="0.30366868036982314"/>
+          <c:h val="3.6329640710949886E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4533,7 +4551,7 @@
   <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4570,7 +4588,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>

</xml_diff>